<commit_message>
add: se agregan las ubicaciones y se arreglan bugs
</commit_message>
<xml_diff>
--- a/db/populationQueries/actividades_economicas.xlsx
+++ b/db/populationQueries/actividades_economicas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\Trabajo\automata_qr_payments\db\populationQueries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53A0A38-1FC0-4C32-B9D6-CBB455CA377D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06929C1B-7C6C-4E87-A932-E4068857CAAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3059,8 +3059,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B715"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A423" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B427" sqref="B427"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>